<commit_message>
Starting fix on split plot analysis
Error found by Zhimin Pan
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/ROC/rocSpA.xlsx
+++ b/inst/extdata/toyFiles/ROC/rocSpA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27116"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/ROC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigi\Documents\PHD-2021\mrmc\01. 学习\a1.多中心\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0996976-A3DA-8C4B-A19F-8317267B63B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29EDF44-9F90-41F4-A72D-A2A59C5A388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="2160" windowWidth="10580" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="756" windowWidth="22560" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="18">
   <si>
     <t>CaseID</t>
   </si>
@@ -50,19 +44,19 @@
     <t>ModalityID</t>
   </si>
   <si>
+    <t>NL_Rating</t>
+  </si>
+  <si>
+    <t>LL_Rating</t>
+  </si>
+  <si>
     <t>Paradigm</t>
   </si>
   <si>
     <t>ROC</t>
   </si>
   <si>
-    <t>split-plot-a</t>
-  </si>
-  <si>
     <t>(2)</t>
-  </si>
-  <si>
-    <t>(4)</t>
   </si>
   <si>
     <t>1,  2</t>
@@ -71,17 +65,34 @@
     <t>3,  4</t>
   </si>
   <si>
-    <t>FP_Rating</t>
+    <t>(1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>TP_Rating</t>
+    <t>1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPLIT-PLOT-A</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,6 +116,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,107 +252,107 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="101">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="100" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -631,16 +649,16 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="5" width="8.77734375" style="1"/>
+    <col min="6" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -654,15 +672,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>4</v>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>16</v>
@@ -670,16 +688,16 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>17</v>
@@ -687,16 +705,16 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>4</v>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>18</v>
@@ -708,12 +726,12 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>19</v>
@@ -725,12 +743,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>4</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
@@ -742,12 +760,12 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>4</v>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>16</v>
@@ -759,12 +777,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>4</v>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="1">
         <v>17</v>
@@ -776,12 +794,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>18</v>
@@ -793,12 +811,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>4</v>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>19</v>
@@ -810,12 +828,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
-        <v>4</v>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>20</v>
@@ -827,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -840,11 +858,11 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -857,11 +875,11 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -878,7 +896,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -895,7 +913,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -912,7 +930,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -929,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -946,7 +964,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -963,7 +981,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -980,7 +998,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -998,6 +1016,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -1013,16 +1032,16 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="4" width="8.77734375" style="1"/>
+    <col min="5" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1033,15 +1052,15 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>4</v>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>6</v>
@@ -1051,12 +1070,12 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>7</v>
@@ -1066,12 +1085,12 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>4</v>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
@@ -1081,12 +1100,12 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>9</v>
@@ -1096,12 +1115,12 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>4</v>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>10</v>
@@ -1111,12 +1130,12 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>4</v>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -1126,12 +1145,12 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="1">
-        <v>4</v>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -1141,12 +1160,12 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="1">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -1156,12 +1175,12 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>4</v>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -1171,12 +1190,12 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="1">
-        <v>4</v>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
@@ -1186,7 +1205,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1201,7 +1220,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1216,7 +1235,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -1231,7 +1250,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1246,7 +1265,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1261,7 +1280,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -1276,7 +1295,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -1291,7 +1310,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -1306,7 +1325,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -1321,7 +1340,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -1337,6 +1356,7 @@
       <c r="E21" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
@@ -1352,19 +1372,19 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D21"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="8.77734375" style="1"/>
+    <col min="4" max="4" width="9.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1381,10 +1401,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -1398,13 +1418,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>7</v>
       </c>
@@ -1418,13 +1438,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -1438,10 +1458,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -1455,10 +1475,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -1472,10 +1492,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -1489,10 +1509,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>17</v>
       </c>
@@ -1506,10 +1526,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>18</v>
       </c>
@@ -1523,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -1540,10 +1560,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>20</v>
       </c>
@@ -1557,10 +1577,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1574,10 +1594,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -1591,10 +1611,10 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1608,10 +1628,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1625,10 +1645,10 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -1642,10 +1662,10 @@
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1659,10 +1679,10 @@
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1676,10 +1696,10 @@
         <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1693,10 +1713,10 @@
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1710,10 +1730,10 @@
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1727,14 +1747,15 @@
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="E12:E21 E2:E11" numberStoredAsText="1"/>
+    <ignoredError sqref="E12:E21" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>